<commit_message>
memperbaiki dan tambhan birthday di reminder
</commit_message>
<xml_diff>
--- a/public/reminder/format.xlsx
+++ b/public/reminder/format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/s2p-project/s2p-helper/public/reminder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA649594-DE52-8446-8382-6E259BF922A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{403B619C-A9C2-3A4D-AB1F-FC40CD06A805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16160" xr2:uid="{74986FC7-280C-B44C-8A98-DEF5082C173C}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15060" xr2:uid="{4329FB97-11A5-814D-B9D8-9720C8D51466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Sampai</t>
+  </si>
   <si>
     <t>Dari</t>
   </si>
   <si>
-    <t>Sampai</t>
-  </si>
-  <si>
     <t>Expired</t>
   </si>
   <si>
@@ -51,16 +57,13 @@
   </si>
   <si>
     <t>Deskripsi</t>
-  </si>
-  <si>
-    <t>Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,13 +71,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,14 +103,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,44 +428,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671828D1-C5EA-F74B-B9A1-EB82E60A54F9}">
-  <dimension ref="B1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0FE4BF-F61A-5147-ADAE-6274DFBADF90}">
+  <dimension ref="B1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="2:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E2" s="1"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moduk Reminder : memperbaiki typo di reminder
</commit_message>
<xml_diff>
--- a/public/reminder/format.xlsx
+++ b/public/reminder/format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/s2p-project/s2p-helper/public/reminder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/support/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{403B619C-A9C2-3A4D-AB1F-FC40CD06A805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3945E8A-1648-234D-9DB0-6DB9E3499886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15060" xr2:uid="{4329FB97-11A5-814D-B9D8-9720C8D51466}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Type</t>
   </si>
@@ -57,13 +57,16 @@
   </si>
   <si>
     <t>Deskripsi</t>
+  </si>
+  <si>
+    <t>*Note Type =&gt; General / Birthday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,6 +78,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,13 +118,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0FE4BF-F61A-5147-ADAE-6274DFBADF90}">
-  <dimension ref="B1:I2"/>
+  <dimension ref="B1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,10 +456,11 @@
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="29.83203125" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="11" max="11" width="29" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -473,9 +486,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G2" s="1"/>
       <c r="H2" s="3"/>
+      <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modul reminder : perbaikan format excel
</commit_message>
<xml_diff>
--- a/public/reminder/format.xlsx
+++ b/public/reminder/format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/support/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3945E8A-1648-234D-9DB0-6DB9E3499886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0156EA-973B-F94C-B3F9-102357B2E5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15060" xr2:uid="{4329FB97-11A5-814D-B9D8-9720C8D51466}"/>
   </bookViews>
@@ -41,25 +41,25 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Sampai</t>
-  </si>
-  <si>
-    <t>Dari</t>
-  </si>
-  <si>
-    <t>Expired</t>
-  </si>
-  <si>
-    <t>Pengingat</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Deskripsi</t>
-  </si>
-  <si>
     <t>*Note Type =&gt; General / Birthday</t>
+  </si>
+  <si>
+    <t>Validity From</t>
+  </si>
+  <si>
+    <t>Expired Date</t>
+  </si>
+  <si>
+    <t>Reminder Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Validity To</t>
   </si>
 </sst>
 </file>
@@ -441,14 +441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0FE4BF-F61A-5147-ADAE-6274DFBADF90}">
-  <dimension ref="B1:K2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
@@ -460,7 +461,7 @@
     <col min="13" max="13" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,30 +469,33 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="3"/>
-      <c r="K2" s="4" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modul reminder : memperbaiki format
</commit_message>
<xml_diff>
--- a/public/reminder/format.xlsx
+++ b/public/reminder/format.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/support/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/s2p-project/s2p-helper/public/reminder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0156EA-973B-F94C-B3F9-102357B2E5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986C94B9-1C21-3A40-B76A-93653DB2817A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15060" xr2:uid="{4329FB97-11A5-814D-B9D8-9720C8D51466}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4329FB97-11A5-814D-B9D8-9720C8D51466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Type</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>*Note Type =&gt; General / Birthday</t>
-  </si>
-  <si>
-    <t>Validity From</t>
-  </si>
-  <si>
     <t>Expired Date</t>
   </si>
   <si>
@@ -59,14 +53,23 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Validity To</t>
+    <t>Validity From               (Date)</t>
+  </si>
+  <si>
+    <t>Validity To                  (Date)</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Birthday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,17 +78,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
-      <color theme="4"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,12 +95,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,22 +107,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,63 +454,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0FE4BF-F61A-5147-ADAE-6274DFBADF90}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="29.83203125" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="10" max="10" width="13" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="40" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
+      <c r="K1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
-    </row>
+    <row r="2" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{1FEAA4A1-D156-3C4F-AAD9-F404F56EDF3E}">
+      <formula1>$J$1:$K$1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modul Informasi : Menambahkan Form Slip Gaji dan Rekening
</commit_message>
<xml_diff>
--- a/public/reminder/format.xlsx
+++ b/public/reminder/format.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/support/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\s2p-helper\s2p-helper\public\reminder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0156EA-973B-F94C-B3F9-102357B2E5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15060" xr2:uid="{4329FB97-11A5-814D-B9D8-9720C8D51466}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Subject</t>
   </si>
@@ -44,29 +40,27 @@
     <t>Email</t>
   </si>
   <si>
-    <t>*Note Type =&gt; General / Birthday</t>
-  </si>
-  <si>
-    <t>Validity From</t>
-  </si>
-  <si>
-    <t>Expired Date</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Validity To 
+(Date)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expired Date </t>
   </si>
   <si>
     <t>Reminder Date</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Validity To</t>
+    <t>Validity From      (Date)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,17 +69,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
-      <color theme="4"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,21 +100,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,64 +424,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0FE4BF-F61A-5147-ADAE-6274DFBADF90}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="29.83203125" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="5" width="18.75" customWidth="1"/>
+    <col min="6" max="6" width="29.875" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modul Pengumuman & Slip Gaji : Enkripsi data user jakarta cilacap, penutupan akses administrator ke manage slip gaji
</commit_message>
<xml_diff>
--- a/public/reminder/format.xlsx
+++ b/public/reminder/format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/s2p-project/s2p-helper/public/reminder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/support/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E54C94A-1ADC-DC4C-9094-A7BF34A78EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C024B6-CCE1-B144-AC84-0EE1D0AC048E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{4329FB97-11A5-814D-B9D8-9720C8D51466}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Type</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Birthday</t>
+  </si>
+  <si>
+    <t>Email 2</t>
+  </si>
+  <si>
+    <t>Email 3</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0FE4BF-F61A-5147-ADAE-6274DFBADF90}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -468,14 +474,14 @@
     <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.83203125" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="10" max="10" width="13" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="7" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="31.5" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" customWidth="1"/>
+    <col min="12" max="12" width="23" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="40" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -498,20 +504,26 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{1FEAA4A1-D156-3C4F-AAD9-F404F56EDF3E}">
-      <formula1>$J$1:$K$1</formula1>
+      <formula1>$L$1:$M$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>